<commit_message>
split .html files into .css and .js files. add function to ask user if they want to save/load {name}'s rankings.
</commit_message>
<xml_diff>
--- a/user_rankings/Nick_rankings.xlsx
+++ b/user_rankings/Nick_rankings.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dune: Part Two</t>
+          <t>Blade Runner 2049</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Blade Runner 2049</t>
+          <t>Memento</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Blade Runner</t>
+          <t>American Beauty</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Memento</t>
+          <t>Barbie</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>American Beauty</t>
+          <t>Dune: Part Two</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Barbie</t>
+          <t>Big Short, The</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Big Short, The</t>
+          <t>Zodiac</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Zodiac</t>
+          <t>Monty Python and the Holy Grail</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Monty Python and the Holy Grail</t>
+          <t>Everything Everywhere All At Once</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Apocalypse Now</t>
+          <t>Children of Men</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Everything Everywhere All At Once</t>
+          <t>Fifth Element, The</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Children of Men</t>
+          <t>Blade Runner</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Fifth Element, The</t>
+          <t>Sicario</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sicario</t>
+          <t>Last Duel, The</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Last Duel, The</t>
+          <t>Akira</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Akira</t>
+          <t>My Cousin Vinney</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>My Cousin Vinney</t>
+          <t>Others, The</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Others, The</t>
+          <t>Batman</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Batman</t>
+          <t>Batman and Robin</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Batman and Robin</t>
+          <t>Beautiful Mind, A</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Beautiful Mind, A</t>
+          <t>Nice Guys, The</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Nice Guys, The</t>
+          <t>Once Upon a Time... in Hollywood</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Blazing Saddles</t>
+          <t>Indiana Jones and the Last Crusade</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Once Upon a Time... in Hollywood</t>
+          <t>Collateral</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Bullett Train</t>
+          <t>Mad Max: Fury Road</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Collateral</t>
+          <t>Crouching Tiger Hidden Dragon</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Reality Bites</t>
+          <t>Baby Driver</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Crouching Tiger Hidden Dragon</t>
+          <t>Ghost In the Shell</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Baby Driver</t>
+          <t>What We Do in the Shadows</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ghost In the Shell</t>
+          <t>Only Lovers Left Alive</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Only Lovers Left Alive</t>
+          <t>Ghostbusters</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ghostbusters</t>
+          <t>Bullett Train</t>
         </is>
       </c>
     </row>
@@ -841,7 +841,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Indiana Jones and the Last Crusade</t>
+          <t>Reality Bites</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Mad Max: Fury Road</t>
+          <t>Blazing Saddles</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>What We Do in the Shadows</t>
+          <t>Pitch Black</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Pitch Black</t>
+          <t>Robin Hood: Prince of Thieves</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Robin Hood: Prince of Thieves</t>
+          <t>Legend of the Eight Samurai</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Legend of the Eight Samurai</t>
+          <t>Showdown in Little Tokyo</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Showdown in Little Tokyo</t>
+          <t>Lone Wolf and Cub: Baby Cart at the River Styx</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Lone Wolf and Cub: Baby Cart at the River Styx</t>
+          <t>So I Married An Axe Murderer</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>So I Married An Axe Murderer</t>
+          <t>Princess Mononoke</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Princess Mononoke</t>
+          <t>Spartacus</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Spartacus</t>
+          <t>Naked Gun, The</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Naked Gun, The</t>
+          <t>Death Proof</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Death Proof</t>
+          <t>Speed Racer</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Speed Racer</t>
+          <t>Detroit Rock City</t>
         </is>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Detroit Rock City</t>
+          <t>Adventures of Robin Hood, The</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Adventures of Robin Hood, The</t>
+          <t>Flow</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Flow</t>
+          <t>Dr. Strangelove</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Dr. Strangelove</t>
+          <t>To Leslie</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>To Leslie</t>
+          <t>Rashomon</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Rashomon</t>
+          <t>Harakiri</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Harakiri</t>
+          <t>Ed Wood</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Ed Wood</t>
+          <t>Eurovision: The Story of Fire Saga</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Eurovision: The Story of Fire Saga</t>
+          <t>American Gangster</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>American Gangster</t>
+          <t>Vertigo</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Vertigo</t>
+          <t>Fistful of Dollars, A</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Fistful of Dollars, A</t>
+          <t>Lost Highway</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Lost Highway</t>
+          <t>Three Thousand Years of Longing</t>
         </is>
       </c>
     </row>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Three Thousand Years of Longing</t>
+          <t>Mask of Zorro</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Mask of Zorro</t>
+          <t>Bend It Like Beckham</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Bend It Like Beckham</t>
+          <t>Legend</t>
         </is>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Legend</t>
+          <t>But I'm a Cheerleader</t>
         </is>
       </c>
     </row>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>But I'm a Cheerleader</t>
+          <t>13 Assassins</t>
         </is>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Big Trouble in Little China</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>To Sir, With Love</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Whatever Happened to Susan Jane?</t>
+          <t>To Sir, With Love</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Naked Lunch</t>
+          <t>Whatever Happened to Susan Jane?</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>13 Assassins</t>
+          <t>Naked Lunch</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,17 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Big Trouble in Little China</t>
+          <t>Apocalypse Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Interstellar</t>
         </is>
       </c>
     </row>

</xml_diff>